<commit_message>
Updated run to resolve discrepancy for model 2 run vs history plot
</commit_message>
<xml_diff>
--- a/DriverDrowsiness/results/output_ff.xlsx
+++ b/DriverDrowsiness/results/output_ff.xlsx
@@ -561,10 +561,10 @@
         <v>16</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9791666865348816</v>
+        <v>0.9624999761581421</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8999999761581421</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N2" t="n">
         <v>3.196109771728516</v>
@@ -629,7 +629,7 @@
         <v>0.981249988079071</v>
       </c>
       <c r="M3" t="n">
-        <v>0.949999988079071</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N3" t="n">
         <v>3.196109771728516</v>
@@ -691,10 +691,10 @@
         <v>64</v>
       </c>
       <c r="L4" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8999999761581421</v>
+        <v>0.8833333253860474</v>
       </c>
       <c r="N4" t="n">
         <v>3.196109771728516</v>
@@ -756,10 +756,10 @@
         <v>16</v>
       </c>
       <c r="L5" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N5" t="n">
         <v>3.196109771728516</v>
@@ -821,7 +821,7 @@
         <v>32</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9854166507720947</v>
       </c>
       <c r="M6" t="n">
         <v>0.9333333373069763</v>
@@ -886,10 +886,10 @@
         <v>64</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.9791666865348816</v>
       </c>
       <c r="M7" t="n">
-        <v>0.9833333492279053</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
         <v>3.196109771728516</v>
@@ -951,10 +951,10 @@
         <v>16</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9708333611488342</v>
       </c>
       <c r="M8" t="n">
-        <v>0.5333333611488342</v>
+        <v>0.8666666746139526</v>
       </c>
       <c r="N8" t="n">
         <v>1.617740631103516</v>
@@ -1019,7 +1019,7 @@
         <v>0.9770833253860474</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.8833333253860474</v>
       </c>
       <c r="N9" t="n">
         <v>1.617740631103516</v>
@@ -1081,10 +1081,10 @@
         <v>64</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M10" t="n">
-        <v>0.6666666865348816</v>
+        <v>0.9166666865348816</v>
       </c>
       <c r="N10" t="n">
         <v>1.617740631103516</v>
@@ -1146,10 +1146,10 @@
         <v>16</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.9770833253860474</v>
       </c>
       <c r="M11" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N11" t="n">
         <v>1.617740631103516</v>
@@ -1211,10 +1211,10 @@
         <v>32</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.9854166507720947</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5333333611488342</v>
+        <v>0.8833333253860474</v>
       </c>
       <c r="N12" t="n">
         <v>1.617740631103516</v>
@@ -1276,10 +1276,10 @@
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9854166507720947</v>
       </c>
       <c r="M13" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N13" t="n">
         <v>1.617740631103516</v>
@@ -1341,10 +1341,10 @@
         <v>16</v>
       </c>
       <c r="L14" t="n">
+        <v>0.9895833134651184</v>
+      </c>
+      <c r="M14" t="n">
         <v>0.9833333492279053</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.9333333373069763</v>
       </c>
       <c r="N14" t="n">
         <v>3.177555084228516</v>
@@ -1406,10 +1406,10 @@
         <v>32</v>
       </c>
       <c r="L15" t="n">
-        <v>0.9791666865348816</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M15" t="n">
-        <v>0.800000011920929</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N15" t="n">
         <v>3.177555084228516</v>
@@ -1471,10 +1471,10 @@
         <v>64</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9916666746139526</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M16" t="n">
-        <v>0.6499999761581421</v>
+        <v>0.8166666626930237</v>
       </c>
       <c r="N16" t="n">
         <v>3.177555084228516</v>
@@ -1601,10 +1601,10 @@
         <v>32</v>
       </c>
       <c r="L18" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M18" t="n">
-        <v>0.9666666388511658</v>
+        <v>1</v>
       </c>
       <c r="N18" t="n">
         <v>3.177555084228516</v>
@@ -1666,10 +1666,10 @@
         <v>64</v>
       </c>
       <c r="L19" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9916666746139526</v>
       </c>
       <c r="M19" t="n">
-        <v>0.8166666626930237</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="N19" t="n">
         <v>3.177555084228516</v>
@@ -1731,10 +1731,10 @@
         <v>16</v>
       </c>
       <c r="L20" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.9791666865348816</v>
       </c>
       <c r="M20" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N20" t="n">
         <v>1.599185943603516</v>
@@ -1796,7 +1796,7 @@
         <v>32</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M21" t="n">
         <v>1</v>
@@ -1861,10 +1861,10 @@
         <v>64</v>
       </c>
       <c r="L22" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M22" t="n">
-        <v>0.7666666507720947</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N22" t="n">
         <v>1.599185943603516</v>
@@ -1926,10 +1926,10 @@
         <v>16</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9708333611488342</v>
       </c>
       <c r="M23" t="n">
-        <v>0.8999999761581421</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N23" t="n">
         <v>1.599185943603516</v>
@@ -1991,7 +1991,7 @@
         <v>32</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.9791666865348816</v>
       </c>
       <c r="M24" t="n">
         <v>1</v>
@@ -2056,10 +2056,10 @@
         <v>64</v>
       </c>
       <c r="L25" t="n">
-        <v>0.9916666746139526</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M25" t="n">
-        <v>1</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N25" t="n">
         <v>1.599185943603516</v>
@@ -2121,10 +2121,10 @@
         <v>16</v>
       </c>
       <c r="L26" t="n">
-        <v>0.9791666865348816</v>
+        <v>0.9729166626930237</v>
       </c>
       <c r="M26" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N26" t="n">
         <v>1.621250152587891</v>
@@ -2186,10 +2186,10 @@
         <v>32</v>
       </c>
       <c r="L27" t="n">
-        <v>0.9791666865348816</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M27" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N27" t="n">
         <v>1.621250152587891</v>
@@ -2251,10 +2251,10 @@
         <v>64</v>
       </c>
       <c r="L28" t="n">
-        <v>0.9937499761581421</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M28" t="n">
-        <v>0.8333333134651184</v>
+        <v>0.6333333253860474</v>
       </c>
       <c r="N28" t="n">
         <v>1.621250152587891</v>
@@ -2316,10 +2316,10 @@
         <v>16</v>
       </c>
       <c r="L29" t="n">
+        <v>0.9937499761581421</v>
+      </c>
+      <c r="M29" t="n">
         <v>0.9833333492279053</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0.8999999761581421</v>
       </c>
       <c r="N29" t="n">
         <v>1.621250152587891</v>
@@ -2381,10 +2381,10 @@
         <v>32</v>
       </c>
       <c r="L30" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M30" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N30" t="n">
         <v>1.621250152587891</v>
@@ -2446,10 +2446,10 @@
         <v>64</v>
       </c>
       <c r="L31" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M31" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.8166666626930237</v>
       </c>
       <c r="N31" t="n">
         <v>1.621250152587891</v>
@@ -2511,10 +2511,10 @@
         <v>16</v>
       </c>
       <c r="L32" t="n">
-        <v>0.9708333611488342</v>
+        <v>0.9770833253860474</v>
       </c>
       <c r="M32" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N32" t="n">
         <v>0.8241310119628906</v>
@@ -2576,10 +2576,10 @@
         <v>32</v>
       </c>
       <c r="L33" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.9729166626930237</v>
       </c>
       <c r="M33" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N33" t="n">
         <v>0.8241310119628906</v>
@@ -2641,10 +2641,10 @@
         <v>64</v>
       </c>
       <c r="L34" t="n">
-        <v>0.981249988079071</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M34" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N34" t="n">
         <v>0.8241310119628906</v>
@@ -2706,10 +2706,10 @@
         <v>16</v>
       </c>
       <c r="L35" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9916666746139526</v>
       </c>
       <c r="M35" t="n">
-        <v>0.949999988079071</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N35" t="n">
         <v>0.8241310119628906</v>
@@ -2771,7 +2771,7 @@
         <v>32</v>
       </c>
       <c r="L36" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="M36" t="n">
         <v>0.9166666865348816</v>
@@ -2836,10 +2836,10 @@
         <v>64</v>
       </c>
       <c r="L37" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M37" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N37" t="n">
         <v>0.8241310119628906</v>
@@ -2966,7 +2966,7 @@
         <v>32</v>
       </c>
       <c r="L39" t="n">
-        <v>0.981249988079071</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="M39" t="n">
         <v>0.8833333253860474</v>
@@ -3031,10 +3031,10 @@
         <v>64</v>
       </c>
       <c r="L40" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9916666746139526</v>
       </c>
       <c r="M40" t="n">
-        <v>0.8333333134651184</v>
+        <v>0.8833333253860474</v>
       </c>
       <c r="N40" t="n">
         <v>1.610507965087891</v>
@@ -3096,7 +3096,7 @@
         <v>16</v>
       </c>
       <c r="L41" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.9854166507720947</v>
       </c>
       <c r="M41" t="n">
         <v>0.9833333492279053</v>
@@ -3161,7 +3161,7 @@
         <v>32</v>
       </c>
       <c r="L42" t="n">
-        <v>0.9916666746139526</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M42" t="n">
         <v>0.9833333492279053</v>
@@ -3226,10 +3226,10 @@
         <v>64</v>
       </c>
       <c r="L43" t="n">
-        <v>0.9916666746139526</v>
+        <v>1</v>
       </c>
       <c r="M43" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N43" t="n">
         <v>1.610507965087891</v>
@@ -3291,10 +3291,10 @@
         <v>16</v>
       </c>
       <c r="L44" t="n">
-        <v>0.9520833492279053</v>
+        <v>0.9604166746139526</v>
       </c>
       <c r="M44" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.8333333134651184</v>
       </c>
       <c r="N44" t="n">
         <v>0.8133888244628906</v>
@@ -3359,7 +3359,7 @@
         <v>0.9791666865348816</v>
       </c>
       <c r="M45" t="n">
-        <v>1</v>
+        <v>0.8833333253860474</v>
       </c>
       <c r="N45" t="n">
         <v>0.8133888244628906</v>
@@ -3421,10 +3421,10 @@
         <v>64</v>
       </c>
       <c r="L46" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="M46" t="n">
-        <v>0.7333333492279053</v>
+        <v>0.6833333373069763</v>
       </c>
       <c r="N46" t="n">
         <v>0.8133888244628906</v>
@@ -3486,10 +3486,10 @@
         <v>16</v>
       </c>
       <c r="L47" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.96875</v>
       </c>
       <c r="M47" t="n">
-        <v>0.8999999761581421</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N47" t="n">
         <v>0.8133888244628906</v>
@@ -3551,10 +3551,10 @@
         <v>32</v>
       </c>
       <c r="L48" t="n">
+        <v>0.9854166507720947</v>
+      </c>
+      <c r="M48" t="n">
         <v>0.9833333492279053</v>
-      </c>
-      <c r="M48" t="n">
-        <v>1</v>
       </c>
       <c r="N48" t="n">
         <v>0.8133888244628906</v>
@@ -3616,7 +3616,7 @@
         <v>64</v>
       </c>
       <c r="L49" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.9979166388511658</v>
       </c>
       <c r="M49" t="n">
         <v>0.9666666388511658</v>
@@ -3681,10 +3681,10 @@
         <v>16</v>
       </c>
       <c r="L50" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.9770833253860474</v>
       </c>
       <c r="M50" t="n">
-        <v>0.9333333373069763</v>
+        <v>1</v>
       </c>
       <c r="N50" t="n">
         <v>3.181461334228516</v>
@@ -3746,10 +3746,10 @@
         <v>32</v>
       </c>
       <c r="L51" t="n">
+        <v>0.9791666865348816</v>
+      </c>
+      <c r="M51" t="n">
         <v>0.9833333492279053</v>
-      </c>
-      <c r="M51" t="n">
-        <v>0.9666666388511658</v>
       </c>
       <c r="N51" t="n">
         <v>3.181461334228516</v>
@@ -3811,10 +3811,10 @@
         <v>64</v>
       </c>
       <c r="L52" t="n">
-        <v>0.9937499761581421</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M52" t="n">
-        <v>0.6166666746139526</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N52" t="n">
         <v>3.181461334228516</v>
@@ -3876,10 +3876,10 @@
         <v>16</v>
       </c>
       <c r="L53" t="n">
-        <v>0.9791666865348816</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M53" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N53" t="n">
         <v>3.181461334228516</v>
@@ -3941,10 +3941,10 @@
         <v>32</v>
       </c>
       <c r="L54" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9958333373069763</v>
       </c>
       <c r="M54" t="n">
-        <v>0.7166666388511658</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N54" t="n">
         <v>3.181461334228516</v>
@@ -4009,7 +4009,7 @@
         <v>0.9895833134651184</v>
       </c>
       <c r="M55" t="n">
-        <v>1</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N55" t="n">
         <v>3.181461334228516</v>
@@ -4071,10 +4071,10 @@
         <v>16</v>
       </c>
       <c r="L56" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.9729166626930237</v>
       </c>
       <c r="M56" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N56" t="n">
         <v>1.603092193603516</v>
@@ -4136,10 +4136,10 @@
         <v>32</v>
       </c>
       <c r="L57" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.9750000238418579</v>
       </c>
       <c r="M57" t="n">
-        <v>0.9166666865348816</v>
+        <v>1</v>
       </c>
       <c r="N57" t="n">
         <v>1.603092193603516</v>
@@ -4201,10 +4201,10 @@
         <v>64</v>
       </c>
       <c r="L58" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="M58" t="n">
-        <v>1</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N58" t="n">
         <v>1.603092193603516</v>
@@ -4266,10 +4266,10 @@
         <v>16</v>
       </c>
       <c r="L59" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M59" t="n">
-        <v>0.949999988079071</v>
+        <v>1</v>
       </c>
       <c r="N59" t="n">
         <v>1.603092193603516</v>
@@ -4331,10 +4331,10 @@
         <v>32</v>
       </c>
       <c r="L60" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M60" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N60" t="n">
         <v>1.603092193603516</v>
@@ -4399,7 +4399,7 @@
         <v>0.9791666865348816</v>
       </c>
       <c r="M61" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.699999988079071</v>
       </c>
       <c r="N61" t="n">
         <v>1.603092193603516</v>
@@ -4461,7 +4461,7 @@
         <v>16</v>
       </c>
       <c r="L62" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9791666865348816</v>
       </c>
       <c r="M62" t="n">
         <v>0.8999999761581421</v>
@@ -4526,10 +4526,10 @@
         <v>32</v>
       </c>
       <c r="L63" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M63" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.8666666746139526</v>
       </c>
       <c r="N63" t="n">
         <v>3.172183990478516</v>
@@ -4591,10 +4591,10 @@
         <v>64</v>
       </c>
       <c r="L64" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.9916666746139526</v>
       </c>
       <c r="M64" t="n">
-        <v>0.75</v>
+        <v>0.5666666626930237</v>
       </c>
       <c r="N64" t="n">
         <v>3.172183990478516</v>
@@ -4656,10 +4656,10 @@
         <v>16</v>
       </c>
       <c r="L65" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.987500011920929</v>
       </c>
       <c r="M65" t="n">
-        <v>0.8333333134651184</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N65" t="n">
         <v>3.172183990478516</v>
@@ -4721,10 +4721,10 @@
         <v>32</v>
       </c>
       <c r="L66" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M66" t="n">
-        <v>0.8500000238418579</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N66" t="n">
         <v>3.172183990478516</v>
@@ -4786,10 +4786,10 @@
         <v>64</v>
       </c>
       <c r="L67" t="n">
-        <v>0.9958333373069763</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M67" t="n">
-        <v>0.8333333134651184</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N67" t="n">
         <v>3.172183990478516</v>
@@ -4851,10 +4851,10 @@
         <v>16</v>
       </c>
       <c r="L68" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9624999761581421</v>
       </c>
       <c r="M68" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9333333373069763</v>
       </c>
       <c r="N68" t="n">
         <v>1.593814849853516</v>
@@ -4916,10 +4916,10 @@
         <v>32</v>
       </c>
       <c r="L69" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M69" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N69" t="n">
         <v>1.593814849853516</v>
@@ -4984,7 +4984,7 @@
         <v>0.9708333611488342</v>
       </c>
       <c r="M70" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N70" t="n">
         <v>1.593814849853516</v>
@@ -5046,10 +5046,10 @@
         <v>16</v>
       </c>
       <c r="L71" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.9854166507720947</v>
       </c>
       <c r="M71" t="n">
-        <v>0.6833333373069763</v>
+        <v>0.9166666865348816</v>
       </c>
       <c r="N71" t="n">
         <v>1.593814849853516</v>
@@ -5111,7 +5111,7 @@
         <v>32</v>
       </c>
       <c r="L72" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M72" t="n">
         <v>0.9833333492279053</v>
@@ -5176,10 +5176,10 @@
         <v>64</v>
       </c>
       <c r="L73" t="n">
-        <v>0.9958333373069763</v>
+        <v>0.9750000238418579</v>
       </c>
       <c r="M73" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.8833333253860474</v>
       </c>
       <c r="N73" t="n">
         <v>1.593814849853516</v>
@@ -5241,10 +5241,10 @@
         <v>16</v>
       </c>
       <c r="L74" t="n">
-        <v>0.9729166626930237</v>
+        <v>0.96875</v>
       </c>
       <c r="M74" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N74" t="n">
         <v>1.612705230712891</v>
@@ -5306,10 +5306,10 @@
         <v>32</v>
       </c>
       <c r="L75" t="n">
-        <v>0.9958333373069763</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M75" t="n">
-        <v>0.949999988079071</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="N75" t="n">
         <v>1.612705230712891</v>
@@ -5371,10 +5371,10 @@
         <v>64</v>
       </c>
       <c r="L76" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M76" t="n">
-        <v>0.75</v>
+        <v>0.8333333134651184</v>
       </c>
       <c r="N76" t="n">
         <v>1.612705230712891</v>
@@ -5436,10 +5436,10 @@
         <v>16</v>
       </c>
       <c r="L77" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.96875</v>
       </c>
       <c r="M77" t="n">
-        <v>1</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N77" t="n">
         <v>1.612705230712891</v>
@@ -5501,10 +5501,10 @@
         <v>32</v>
       </c>
       <c r="L78" t="n">
-        <v>0.987500011920929</v>
+        <v>0.9937499761581421</v>
       </c>
       <c r="M78" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N78" t="n">
         <v>1.612705230712891</v>
@@ -5569,7 +5569,7 @@
         <v>0.9916666746139526</v>
       </c>
       <c r="M79" t="n">
-        <v>0.949999988079071</v>
+        <v>0.9166666865348816</v>
       </c>
       <c r="N79" t="n">
         <v>1.612705230712891</v>
@@ -5631,7 +5631,7 @@
         <v>16</v>
       </c>
       <c r="L80" t="n">
-        <v>0.9624999761581421</v>
+        <v>0.9458333253860474</v>
       </c>
       <c r="M80" t="n">
         <v>1</v>
@@ -5696,10 +5696,10 @@
         <v>32</v>
       </c>
       <c r="L81" t="n">
-        <v>0.9708333611488342</v>
+        <v>0.96875</v>
       </c>
       <c r="M81" t="n">
-        <v>1</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N81" t="n">
         <v>0.8155860900878906</v>
@@ -5761,10 +5761,10 @@
         <v>64</v>
       </c>
       <c r="L82" t="n">
-        <v>0.9708333611488342</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M82" t="n">
-        <v>0.949999988079071</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N82" t="n">
         <v>0.8155860900878906</v>
@@ -5826,10 +5826,10 @@
         <v>16</v>
       </c>
       <c r="L83" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.9729166626930237</v>
       </c>
       <c r="M83" t="n">
-        <v>0.9666666388511658</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N83" t="n">
         <v>0.8155860900878906</v>
@@ -5891,10 +5891,10 @@
         <v>32</v>
       </c>
       <c r="L84" t="n">
-        <v>0.9750000238418579</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M84" t="n">
-        <v>1</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N84" t="n">
         <v>0.8155860900878906</v>
@@ -5956,10 +5956,10 @@
         <v>64</v>
       </c>
       <c r="L85" t="n">
-        <v>0.9854166507720947</v>
+        <v>0.9958333373069763</v>
       </c>
       <c r="M85" t="n">
-        <v>0.949999988079071</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N85" t="n">
         <v>0.8155860900878906</v>
@@ -6021,10 +6021,10 @@
         <v>16</v>
       </c>
       <c r="L86" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9645833373069763</v>
       </c>
       <c r="M86" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N86" t="n">
         <v>1.607334136962891</v>
@@ -6086,10 +6086,10 @@
         <v>32</v>
       </c>
       <c r="L87" t="n">
-        <v>0.9937499761581421</v>
+        <v>0.9854166507720947</v>
       </c>
       <c r="M87" t="n">
-        <v>0.9166666865348816</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N87" t="n">
         <v>1.607334136962891</v>
@@ -6151,7 +6151,7 @@
         <v>64</v>
       </c>
       <c r="L88" t="n">
-        <v>0.9937499761581421</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M88" t="n">
         <v>0.6333333253860474</v>
@@ -6216,7 +6216,7 @@
         <v>16</v>
       </c>
       <c r="L89" t="n">
-        <v>0.96875</v>
+        <v>0.9770833253860474</v>
       </c>
       <c r="M89" t="n">
         <v>0.949999988079071</v>
@@ -6284,7 +6284,7 @@
         <v>0.9895833134651184</v>
       </c>
       <c r="M90" t="n">
-        <v>0.8999999761581421</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N90" t="n">
         <v>1.607334136962891</v>
@@ -6346,10 +6346,10 @@
         <v>64</v>
       </c>
       <c r="L91" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.9979166388511658</v>
       </c>
       <c r="M91" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N91" t="n">
         <v>1.607334136962891</v>
@@ -6411,10 +6411,10 @@
         <v>16</v>
       </c>
       <c r="L92" t="n">
-        <v>0.956250011920929</v>
+        <v>0.9645833373069763</v>
       </c>
       <c r="M92" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="N92" t="n">
         <v>0.8102149963378906</v>
@@ -6476,10 +6476,10 @@
         <v>32</v>
       </c>
       <c r="L93" t="n">
-        <v>0.9895833134651184</v>
+        <v>0.9791666865348816</v>
       </c>
       <c r="M93" t="n">
-        <v>1</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="N93" t="n">
         <v>0.8102149963378906</v>
@@ -6541,10 +6541,10 @@
         <v>64</v>
       </c>
       <c r="L94" t="n">
-        <v>0.9958333373069763</v>
+        <v>0.9791666865348816</v>
       </c>
       <c r="M94" t="n">
-        <v>0.9333333373069763</v>
+        <v>0.9666666388511658</v>
       </c>
       <c r="N94" t="n">
         <v>0.8102149963378906</v>
@@ -6606,7 +6606,7 @@
         <v>16</v>
       </c>
       <c r="L95" t="n">
-        <v>0.9833333492279053</v>
+        <v>0.9895833134651184</v>
       </c>
       <c r="M95" t="n">
         <v>0.9833333492279053</v>
@@ -6671,10 +6671,10 @@
         <v>32</v>
       </c>
       <c r="L96" t="n">
-        <v>0.9770833253860474</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="M96" t="n">
-        <v>0.8333333134651184</v>
+        <v>1</v>
       </c>
       <c r="N96" t="n">
         <v>0.8102149963378906</v>

</xml_diff>